<commit_message>
Can now scalar write values to excel range.
</commit_message>
<xml_diff>
--- a/docs/content/SimpleInvoice.xlsx
+++ b/docs/content/SimpleInvoice.xlsx
@@ -144,6 +144,10 @@
       <x:t xml:space="preserve">
 Thank you for your business!</x:t>
     </x:r>
+  </x:si>
+  <x:si/>
+  <x:si>
+    <x:t>Colin Bull</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -983,7 +987,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B8" s="42" t="s">
-        <x:v>1</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C8" s="42"/>
       <x:c r="E8" s="10"/>

</xml_diff>

<commit_message>
Will now infer types of excel cells if saved in the correct format
</commit_message>
<xml_diff>
--- a/docs/content/SimpleInvoice.xlsx
+++ b/docs/content/SimpleInvoice.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <x:workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Appdev\officeprovider\docs\content\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="-12" yWindow="6168" windowWidth="19176" windowHeight="6228"/>
+    <x:workbookView xWindow="-15" yWindow="6165" windowWidth="19170" windowHeight="6225"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Service Invoice" sheetId="1" r:id="rId1"/>
@@ -29,7 +24,7 @@
     <x:definedName name="Total">'Service Invoice'!$F$41</x:definedName>
     <x:definedName name="VAT">'Service Invoice'!$F$40</x:definedName>
   </x:definedNames>
-  <x:calcPr calcId="152511"/>
+  <x:calcPr calcId="144525"/>
 </x:workbook>
 </file>
 
@@ -145,7 +140,6 @@
 Thank you for your business!</x:t>
     </x:r>
   </x:si>
-  <x:si/>
   <x:si>
     <x:t>Colin Bull</x:t>
   </x:si>
@@ -421,27 +415,41 @@
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -449,23 +457,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,30 +899,30 @@
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:dimension ref="A1:F51"/>
   <x:sheetViews>
-    <x:sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <x:selection activeCell="F41" sqref="F41"/>
+    <x:sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <x:selection activeCell="B8" sqref="B8:C8"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="2" width="13.6640625" style="2" customWidth="1"/>
-    <x:col min="3" max="3" width="21.6640625" style="2" customWidth="1"/>
-    <x:col min="4" max="5" width="13.6640625" style="2" customWidth="1"/>
-    <x:col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
-    <x:col min="7" max="16384" width="9.109375" style="2"/>
+    <x:col min="1" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <x:col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
+    <x:col min="4" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <x:col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
+    <x:col min="7" max="16384" width="9.140625" style="2"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+    <x:row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="1">
       <x:c r="A1" s="1"/>
-      <x:c r="B1" s="46" t="s">
+      <x:c r="B1" s="44" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C1" s="46"/>
-      <x:c r="D1" s="46"/>
-      <x:c r="E1" s="46"/>
-      <x:c r="F1" s="46"/>
-    </x:row>
-    <x:row r="2" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
+      <x:c r="C1" s="44"/>
+      <x:c r="D1" s="44"/>
+      <x:c r="E1" s="44"/>
+      <x:c r="F1" s="44"/>
+    </x:row>
+    <x:row r="2" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A2" s="3"/>
       <x:c r="B2" s="3"/>
       <x:c r="C2" s="3"/>
@@ -936,27 +930,27 @@
       <x:c r="E2" s="5"/>
       <x:c r="F2" s="6"/>
     </x:row>
-    <x:row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <x:c r="A3" s="47" t="s">
+    <x:row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="A3" s="45" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B3" s="47"/>
-      <x:c r="C3" s="47"/>
+      <x:c r="B3" s="45"/>
+      <x:c r="C3" s="45"/>
       <x:c r="D3" s="4"/>
       <x:c r="E3" s="5" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F3" s="6">
         <x:f ca="1">TODAY()</x:f>
-        <x:v>41891</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A4" s="48" t="s">
+        <x:v>41892</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="46" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B4" s="48"/>
-      <x:c r="C4" s="48"/>
+      <x:c r="B4" s="46"/>
+      <x:c r="C4" s="46"/>
       <x:c r="D4" s="7"/>
       <x:c r="E4" s="5" t="s">
         <x:v>23</x:v>
@@ -966,9 +960,9 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="48"/>
-      <x:c r="B5" s="48"/>
-      <x:c r="C5" s="48"/>
+      <x:c r="A5" s="46"/>
+      <x:c r="B5" s="46"/>
+      <x:c r="C5" s="46"/>
       <x:c r="E5" s="5" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -986,19 +980,19 @@
       <x:c r="A8" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B8" s="42" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C8" s="42"/>
+      <x:c r="B8" s="47" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C8" s="47"/>
       <x:c r="E8" s="10"/>
       <x:c r="F8" s="10"/>
     </x:row>
     <x:row r="9" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A9" s="11"/>
-      <x:c r="B9" s="42" t="s">
+      <x:c r="B9" s="47" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C9" s="42"/>
+      <x:c r="C9" s="47"/>
       <x:c r="D9" s="9"/>
       <x:c r="E9" s="10"/>
       <x:c r="F9" s="10"/>
@@ -1034,36 +1028,36 @@
       <x:c r="F12" s="10"/>
     </x:row>
     <x:row r="13" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A13" s="49"/>
-      <x:c r="B13" s="49"/>
-      <x:c r="C13" s="49"/>
-      <x:c r="D13" s="49"/>
-      <x:c r="E13" s="49"/>
-      <x:c r="F13" s="49"/>
-    </x:row>
-    <x:row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A14" s="52"/>
-      <x:c r="B14" s="52"/>
+      <x:c r="A13" s="48"/>
+      <x:c r="B13" s="48"/>
+      <x:c r="C13" s="48"/>
+      <x:c r="D13" s="48"/>
+      <x:c r="E13" s="48"/>
+      <x:c r="F13" s="48"/>
+    </x:row>
+    <x:row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A14" s="38"/>
+      <x:c r="B14" s="38"/>
       <x:c r="C14"/>
-      <x:c r="D14" s="41" t="s">
+      <x:c r="D14" s="39" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E14" s="41"/>
+      <x:c r="E14" s="39"/>
       <x:c r="F14" s="27" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A15" s="52"/>
-      <x:c r="B15" s="52"/>
+    <x:row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A15" s="38"/>
+      <x:c r="B15" s="38"/>
       <x:c r="C15"/>
-      <x:c r="D15" s="38" t="s">
+      <x:c r="D15" s="40" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="E15" s="38"/>
+      <x:c r="E15" s="40"/>
       <x:c r="F15" s="28"/>
     </x:row>
-    <x:row r="16" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="16" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A16" s="12"/>
       <x:c r="B16" s="12"/>
       <x:c r="C16" s="13"/>
@@ -1071,15 +1065,15 @@
       <x:c r="E16" s="13"/>
       <x:c r="F16" s="14"/>
     </x:row>
-    <x:row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="27" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B17" s="41" t="s">
+      <x:c r="B17" s="39" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C17" s="41"/>
-      <x:c r="D17" s="41"/>
+      <x:c r="C17" s="39"/>
+      <x:c r="D17" s="39"/>
       <x:c r="E17" s="27" t="s">
         <x:v>16</x:v>
       </x:c>
@@ -1087,238 +1081,238 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A18" s="29"/>
-      <x:c r="B18" s="37"/>
-      <x:c r="C18" s="38"/>
-      <x:c r="D18" s="38"/>
+      <x:c r="B18" s="43"/>
+      <x:c r="C18" s="40"/>
+      <x:c r="D18" s="40"/>
       <x:c r="E18" s="31"/>
       <x:c r="F18" s="32" t="str">
         <x:f t="shared" ref="F18:F38" si="0">IF(SUM(A18)&gt;0,SUM(A18*E18),"")</x:f>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A19" s="30"/>
-      <x:c r="B19" s="39"/>
-      <x:c r="C19" s="40"/>
-      <x:c r="D19" s="40"/>
+      <x:c r="B19" s="41"/>
+      <x:c r="C19" s="42"/>
+      <x:c r="D19" s="42"/>
       <x:c r="E19" s="33"/>
       <x:c r="F19" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="29"/>
-      <x:c r="B20" s="37"/>
-      <x:c r="C20" s="38"/>
-      <x:c r="D20" s="38"/>
+      <x:c r="B20" s="43"/>
+      <x:c r="C20" s="40"/>
+      <x:c r="D20" s="40"/>
       <x:c r="E20" s="34"/>
       <x:c r="F20" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A21" s="30"/>
-      <x:c r="B21" s="39"/>
-      <x:c r="C21" s="40"/>
-      <x:c r="D21" s="40"/>
+      <x:c r="B21" s="41"/>
+      <x:c r="C21" s="42"/>
+      <x:c r="D21" s="42"/>
       <x:c r="E21" s="33"/>
       <x:c r="F21" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A22" s="29"/>
-      <x:c r="B22" s="37"/>
-      <x:c r="C22" s="38"/>
-      <x:c r="D22" s="38"/>
+      <x:c r="B22" s="43"/>
+      <x:c r="C22" s="40"/>
+      <x:c r="D22" s="40"/>
       <x:c r="E22" s="34"/>
       <x:c r="F22" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A23" s="30"/>
-      <x:c r="B23" s="39"/>
-      <x:c r="C23" s="40"/>
-      <x:c r="D23" s="40"/>
+      <x:c r="B23" s="41"/>
+      <x:c r="C23" s="42"/>
+      <x:c r="D23" s="42"/>
       <x:c r="E23" s="33"/>
       <x:c r="F23" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A24" s="29"/>
-      <x:c r="B24" s="37"/>
-      <x:c r="C24" s="38"/>
-      <x:c r="D24" s="38"/>
+      <x:c r="B24" s="43"/>
+      <x:c r="C24" s="40"/>
+      <x:c r="D24" s="40"/>
       <x:c r="E24" s="34"/>
       <x:c r="F24" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="30"/>
-      <x:c r="B25" s="39"/>
-      <x:c r="C25" s="40"/>
-      <x:c r="D25" s="40"/>
+      <x:c r="B25" s="41"/>
+      <x:c r="C25" s="42"/>
+      <x:c r="D25" s="42"/>
       <x:c r="E25" s="33"/>
       <x:c r="F25" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A26" s="29"/>
-      <x:c r="B26" s="37"/>
-      <x:c r="C26" s="38"/>
-      <x:c r="D26" s="38"/>
+      <x:c r="B26" s="43"/>
+      <x:c r="C26" s="40"/>
+      <x:c r="D26" s="40"/>
       <x:c r="E26" s="34"/>
       <x:c r="F26" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A27" s="30"/>
-      <x:c r="B27" s="39"/>
-      <x:c r="C27" s="40"/>
-      <x:c r="D27" s="40"/>
+      <x:c r="B27" s="41"/>
+      <x:c r="C27" s="42"/>
+      <x:c r="D27" s="42"/>
       <x:c r="E27" s="33"/>
       <x:c r="F27" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A28" s="29"/>
-      <x:c r="B28" s="37"/>
-      <x:c r="C28" s="38"/>
-      <x:c r="D28" s="38"/>
+      <x:c r="B28" s="43"/>
+      <x:c r="C28" s="40"/>
+      <x:c r="D28" s="40"/>
       <x:c r="E28" s="34"/>
       <x:c r="F28" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A29" s="30"/>
-      <x:c r="B29" s="39"/>
-      <x:c r="C29" s="40"/>
-      <x:c r="D29" s="40"/>
+      <x:c r="B29" s="41"/>
+      <x:c r="C29" s="42"/>
+      <x:c r="D29" s="42"/>
       <x:c r="E29" s="33"/>
       <x:c r="F29" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A30" s="29"/>
-      <x:c r="B30" s="37"/>
-      <x:c r="C30" s="38"/>
-      <x:c r="D30" s="38"/>
+      <x:c r="B30" s="43"/>
+      <x:c r="C30" s="40"/>
+      <x:c r="D30" s="40"/>
       <x:c r="E30" s="34"/>
       <x:c r="F30" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A31" s="30"/>
-      <x:c r="B31" s="39"/>
-      <x:c r="C31" s="40"/>
-      <x:c r="D31" s="40"/>
+      <x:c r="B31" s="41"/>
+      <x:c r="C31" s="42"/>
+      <x:c r="D31" s="42"/>
       <x:c r="E31" s="33"/>
       <x:c r="F31" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A32" s="29"/>
-      <x:c r="B32" s="37"/>
-      <x:c r="C32" s="38"/>
-      <x:c r="D32" s="38"/>
+      <x:c r="B32" s="43"/>
+      <x:c r="C32" s="40"/>
+      <x:c r="D32" s="40"/>
       <x:c r="E32" s="34"/>
       <x:c r="F32" s="33" t="str">
         <x:f>IF(SUM(A32)&gt;0,SUM(A32*E32),"")</x:f>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A33" s="30"/>
-      <x:c r="B33" s="39"/>
-      <x:c r="C33" s="40"/>
-      <x:c r="D33" s="40"/>
+      <x:c r="B33" s="41"/>
+      <x:c r="C33" s="42"/>
+      <x:c r="D33" s="42"/>
       <x:c r="E33" s="33"/>
       <x:c r="F33" s="33" t="str">
         <x:f>IF(SUM(A33)&gt;0,SUM(A33*E33),"")</x:f>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A34" s="29"/>
-      <x:c r="B34" s="37"/>
-      <x:c r="C34" s="38"/>
-      <x:c r="D34" s="38"/>
+      <x:c r="B34" s="43"/>
+      <x:c r="C34" s="40"/>
+      <x:c r="D34" s="40"/>
       <x:c r="E34" s="34"/>
       <x:c r="F34" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A35" s="30"/>
-      <x:c r="B35" s="39"/>
-      <x:c r="C35" s="40"/>
-      <x:c r="D35" s="40"/>
+      <x:c r="B35" s="41"/>
+      <x:c r="C35" s="42"/>
+      <x:c r="D35" s="42"/>
       <x:c r="E35" s="33"/>
       <x:c r="F35" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A36" s="29"/>
-      <x:c r="B36" s="37"/>
-      <x:c r="C36" s="38"/>
-      <x:c r="D36" s="38"/>
+      <x:c r="B36" s="43"/>
+      <x:c r="C36" s="40"/>
+      <x:c r="D36" s="40"/>
       <x:c r="E36" s="34"/>
       <x:c r="F36" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A37" s="30"/>
-      <x:c r="B37" s="39"/>
-      <x:c r="C37" s="40"/>
-      <x:c r="D37" s="40"/>
+      <x:c r="B37" s="41"/>
+      <x:c r="C37" s="42"/>
+      <x:c r="D37" s="42"/>
       <x:c r="E37" s="33"/>
       <x:c r="F37" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A38" s="29"/>
-      <x:c r="B38" s="37"/>
-      <x:c r="C38" s="38"/>
-      <x:c r="D38" s="38"/>
+      <x:c r="B38" s="43"/>
+      <x:c r="C38" s="40"/>
+      <x:c r="D38" s="40"/>
       <x:c r="E38" s="34"/>
       <x:c r="F38" s="33" t="str">
         <x:f t="shared" si="0"/>
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A39" s="16"/>
       <x:c r="B39" s="17"/>
       <x:c r="C39" s="17"/>
@@ -1331,7 +1325,7 @@
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A40" s="17"/>
       <x:c r="B40" s="17"/>
       <x:c r="C40" s="17"/>
@@ -1341,7 +1335,7 @@
       </x:c>
       <x:c r="F40" s="34"/>
     </x:row>
-    <x:row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A41" s="17"/>
       <x:c r="B41" s="17"/>
       <x:c r="C41" s="17"/>
@@ -1354,33 +1348,33 @@
         <x:v/>
       </x:c>
     </x:row>
-    <x:row r="42" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A42" s="43"/>
-      <x:c r="B42" s="43"/>
-      <x:c r="C42" s="43"/>
-      <x:c r="D42" s="43"/>
-      <x:c r="E42" s="43"/>
-      <x:c r="F42" s="43"/>
-    </x:row>
-    <x:row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A43" s="44" t="s">
+    <x:row r="42" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A42" s="49"/>
+      <x:c r="B42" s="49"/>
+      <x:c r="C42" s="49"/>
+      <x:c r="D42" s="49"/>
+      <x:c r="E42" s="49"/>
+      <x:c r="F42" s="49"/>
+    </x:row>
+    <x:row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A43" s="50" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B43" s="45"/>
-      <x:c r="C43" s="45"/>
-      <x:c r="D43" s="45"/>
-      <x:c r="E43" s="45"/>
-      <x:c r="F43" s="45"/>
-    </x:row>
-    <x:row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A44" s="45"/>
-      <x:c r="B44" s="45"/>
-      <x:c r="C44" s="45"/>
-      <x:c r="D44" s="45"/>
-      <x:c r="E44" s="45"/>
-      <x:c r="F44" s="45"/>
-    </x:row>
-    <x:row r="45" spans="1:6" ht="9.9" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="B43" s="51"/>
+      <x:c r="C43" s="51"/>
+      <x:c r="D43" s="51"/>
+      <x:c r="E43" s="51"/>
+      <x:c r="F43" s="51"/>
+    </x:row>
+    <x:row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A44" s="51"/>
+      <x:c r="B44" s="51"/>
+      <x:c r="C44" s="51"/>
+      <x:c r="D44" s="51"/>
+      <x:c r="E44" s="51"/>
+      <x:c r="F44" s="51"/>
+    </x:row>
+    <x:row r="45" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A45" s="19"/>
       <x:c r="B45" s="19"/>
       <x:c r="C45" s="19"/>
@@ -1388,17 +1382,17 @@
       <x:c r="E45" s="19"/>
       <x:c r="F45" s="19"/>
     </x:row>
-    <x:row r="46" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A46" s="36" t="s">
+    <x:row r="46" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <x:c r="A46" s="52" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="B46" s="36"/>
-      <x:c r="C46" s="36"/>
-      <x:c r="D46" s="36"/>
-      <x:c r="E46" s="36"/>
-      <x:c r="F46" s="36"/>
-    </x:row>
-    <x:row r="47" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="B46" s="52"/>
+      <x:c r="C46" s="52"/>
+      <x:c r="D46" s="52"/>
+      <x:c r="E46" s="52"/>
+      <x:c r="F46" s="52"/>
+    </x:row>
+    <x:row r="47" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A47" s="21"/>
       <x:c r="B47" s="22"/>
       <x:c r="C47" s="22"/>
@@ -1406,20 +1400,20 @@
       <x:c r="E47" s="9"/>
       <x:c r="F47" s="9"/>
     </x:row>
-    <x:row r="48" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="B48" s="50"/>
-      <x:c r="C48" s="51"/>
-      <x:c r="D48" s="51"/>
-      <x:c r="E48" s="51"/>
-    </x:row>
-    <x:row r="49" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="48" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="B48" s="36"/>
+      <x:c r="C48" s="37"/>
+      <x:c r="D48" s="37"/>
+      <x:c r="E48" s="37"/>
+    </x:row>
+    <x:row r="49" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="B49" s="24"/>
       <x:c r="C49" s="25"/>
       <x:c r="D49" s="25"/>
       <x:c r="E49" s="25"/>
     </x:row>
-    <x:row r="50" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <x:row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <x:row r="50" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <x:row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <x:c r="A51" s="26"/>
       <x:c r="B51" s="26"/>
       <x:c r="C51" s="26"/>
@@ -1429,6 +1423,26 @@
     </x:row>
   </x:sheetData>
   <x:mergeCells count="36">
+    <x:mergeCell ref="A46:F46"/>
+    <x:mergeCell ref="B34:D34"/>
+    <x:mergeCell ref="B35:D35"/>
+    <x:mergeCell ref="B31:D31"/>
+    <x:mergeCell ref="B30:D30"/>
+    <x:mergeCell ref="B38:D38"/>
+    <x:mergeCell ref="B37:D37"/>
+    <x:mergeCell ref="B32:D32"/>
+    <x:mergeCell ref="B33:D33"/>
+    <x:mergeCell ref="B19:D19"/>
+    <x:mergeCell ref="B17:D17"/>
+    <x:mergeCell ref="B9:C9"/>
+    <x:mergeCell ref="A42:F42"/>
+    <x:mergeCell ref="A43:F44"/>
+    <x:mergeCell ref="B29:D29"/>
+    <x:mergeCell ref="B1:F1"/>
+    <x:mergeCell ref="A3:C3"/>
+    <x:mergeCell ref="A4:C5"/>
+    <x:mergeCell ref="B8:C8"/>
+    <x:mergeCell ref="A13:F13"/>
     <x:mergeCell ref="B48:E48"/>
     <x:mergeCell ref="A14:B14"/>
     <x:mergeCell ref="A15:B15"/>
@@ -1445,26 +1459,6 @@
     <x:mergeCell ref="B24:D24"/>
     <x:mergeCell ref="B23:D23"/>
     <x:mergeCell ref="B22:D22"/>
-    <x:mergeCell ref="B1:F1"/>
-    <x:mergeCell ref="A3:C3"/>
-    <x:mergeCell ref="A4:C5"/>
-    <x:mergeCell ref="B8:C8"/>
-    <x:mergeCell ref="A13:F13"/>
-    <x:mergeCell ref="B19:D19"/>
-    <x:mergeCell ref="B17:D17"/>
-    <x:mergeCell ref="B9:C9"/>
-    <x:mergeCell ref="A42:F42"/>
-    <x:mergeCell ref="A43:F44"/>
-    <x:mergeCell ref="B29:D29"/>
-    <x:mergeCell ref="A46:F46"/>
-    <x:mergeCell ref="B34:D34"/>
-    <x:mergeCell ref="B35:D35"/>
-    <x:mergeCell ref="B31:D31"/>
-    <x:mergeCell ref="B30:D30"/>
-    <x:mergeCell ref="B38:D38"/>
-    <x:mergeCell ref="B37:D37"/>
-    <x:mergeCell ref="B32:D32"/>
-    <x:mergeCell ref="B33:D33"/>
   </x:mergeCells>
   <x:phoneticPr fontId="1" type="noConversion"/>
   <x:printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Can now handle sheets with chartSheets in
</commit_message>
<xml_diff>
--- a/docs/content/SimpleInvoice.xlsx
+++ b/docs/content/SimpleInvoice.xlsx
@@ -4,10 +4,11 @@
   <x:fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <x:workbookPr/>
   <x:bookViews>
-    <x:workbookView xWindow="-15" yWindow="6165" windowWidth="19170" windowHeight="6225"/>
+    <x:workbookView xWindow="-15" yWindow="6165" windowWidth="19170" windowHeight="6225" activeTab="1"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Service Invoice" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Chart1" sheetId="3" r:id="rId2"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="Address2">'Service Invoice'!$B$11</x:definedName>
@@ -29,121 +30,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <x:si>
-    <x:t>[100]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Name]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Company Name]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Street Address]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[City, ST  ZIP Code]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Phone]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[ABC12345]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Due upon receipt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Your Company Name]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date:</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Customer ID:</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Invoice</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Payment Terms</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Due Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Qty</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unit Price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Line Total</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Subtotal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sales Tax</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Total</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Street Address], [City, ST  ZIP Code]  [Phone]  [Fax]  [E-mail]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>To:</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Invoice #:</x:t>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:t xml:space="preserve"> </x:t>
-    </x:r>
-    <x:r>
-      <x:rPr>
-        <x:sz val="8"/>
-        <x:color theme="1" tint="0.249977111117893"/>
-        <x:rFont val="Palatino Linotype"/>
-        <x:family val="1"/>
-        <x:scheme val="minor"/>
-      </x:rPr>
-      <x:t>[Your Company Slogan Here]</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:sz val="8"/>
-        <x:color theme="6"/>
-        <x:rFont val="Palatino Linotype"/>
-        <x:family val="1"/>
-        <x:scheme val="minor"/>
-      </x:rPr>
-      <x:t>Make all checks payable to [Your Company Name]</x:t>
-    </x:r>
-    <x:r>
-      <x:rPr>
-        <x:sz val="10"/>
-        <x:color theme="1" tint="0.249977111117893"/>
-        <x:rFont val="Palatino Linotype"/>
-        <x:family val="1"/>
-        <x:scheme val="minor"/>
-      </x:rPr>
-      <x:t xml:space="preserve">
-Thank you for your business!</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:t>Colin Bull</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>[100]</t>
+  </si>
+  <si>
+    <t>[Company Name]</t>
+  </si>
+  <si>
+    <t>[Street Address]</t>
+  </si>
+  <si>
+    <t>[City, ST  ZIP Code]</t>
+  </si>
+  <si>
+    <t>[Phone]</t>
+  </si>
+  <si>
+    <t>[ABC12345]</t>
+  </si>
+  <si>
+    <t>Due upon receipt</t>
+  </si>
+  <si>
+    <t>[Your Company Name]</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Customer ID:</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Payment Terms</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Line Total</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Sales Tax</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>[Street Address], [City, ST  ZIP Code]  [Phone]  [Fax]  [E-mail]</t>
+  </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>Invoice #:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Your Company Slogan Here]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="6"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Make all checks payable to [Your Company Name]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Thank you for your business!</t>
+    </r>
+  </si>
+  <si>
+    <t>Colin Bull</t>
+  </si>
+  <si>
+    <t>FooBar</t>
+  </si>
+  <si>
+    <t>FooBar 2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,41 +419,27 @@
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -457,9 +447,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,6 +547,158 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Service Invoice'!$A$18:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.00 FooBar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Service Invoice'!$C$18:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="2" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Service Invoice'!$A$19:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.00 FooBar 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Service Invoice'!$C$19:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="2" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="53420416"/>
+        <c:axId val="53421952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="53420416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53421952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="53421952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53420416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,6 +823,33 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9307500" cy="6082500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -899,8 +1082,8 @@
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:dimension ref="A1:F51"/>
   <x:sheetViews>
-    <x:sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <x:selection activeCell="B8" sqref="B8:C8"/>
+    <x:sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <x:selection activeCell="A18" sqref="A18:F19"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -914,13 +1097,13 @@
   <x:sheetData>
     <x:row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="1">
       <x:c r="A1" s="1"/>
-      <x:c r="B1" s="44" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C1" s="44"/>
-      <x:c r="D1" s="44"/>
-      <x:c r="E1" s="44"/>
-      <x:c r="F1" s="44"/>
+      <x:c r="B1" s="46" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C1" s="46"/>
+      <x:c r="D1" s="46"/>
+      <x:c r="E1" s="46"/>
+      <x:c r="F1" s="46"/>
     </x:row>
     <x:row r="2" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A2" s="3"/>
@@ -931,14 +1114,14 @@
       <x:c r="F2" s="6"/>
     </x:row>
     <x:row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="45" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B3" s="45"/>
-      <x:c r="C3" s="45"/>
+      <x:c r="A3" s="47" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="47"/>
+      <x:c r="C3" s="47"/>
       <x:c r="D3" s="4"/>
       <x:c r="E3" s="5" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F3" s="6">
         <x:f ca="1">TODAY()</x:f>
@@ -946,28 +1129,28 @@
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="46" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B4" s="46"/>
-      <x:c r="C4" s="46"/>
+      <x:c r="A4" s="48" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B4" s="48"/>
+      <x:c r="C4" s="48"/>
       <x:c r="D4" s="7"/>
       <x:c r="E4" s="5" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F4" s="5" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="46"/>
-      <x:c r="B5" s="46"/>
-      <x:c r="C5" s="46"/>
+      <x:c r="A5" s="48"/>
+      <x:c r="B5" s="48"/>
+      <x:c r="C5" s="48"/>
       <x:c r="E5" s="5" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F5" s="5" t="s">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -978,21 +1161,21 @@
     </x:row>
     <x:row r="8" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B8" s="47" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C8" s="47"/>
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B8" s="42" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C8" s="42"/>
       <x:c r="E8" s="10"/>
       <x:c r="F8" s="10"/>
     </x:row>
     <x:row r="9" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A9" s="11"/>
-      <x:c r="B9" s="47" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C9" s="47"/>
+      <x:c r="B9" s="42" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C9" s="42"/>
       <x:c r="D9" s="9"/>
       <x:c r="E9" s="10"/>
       <x:c r="F9" s="10"/>
@@ -1000,7 +1183,7 @@
     <x:row r="10" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="9"/>
       <x:c r="B10" s="5" t="s">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C10" s="5"/>
       <x:c r="D10" s="9"/>
@@ -1010,7 +1193,7 @@
     <x:row r="11" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="9"/>
       <x:c r="B11" s="5" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C11" s="5"/>
       <x:c r="D11" s="5"/>
@@ -1020,7 +1203,7 @@
     <x:row r="12" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A12" s="9"/>
       <x:c r="B12" s="5" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C12" s="5"/>
       <x:c r="D12" s="9"/>
@@ -1028,33 +1211,33 @@
       <x:c r="F12" s="10"/>
     </x:row>
     <x:row r="13" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A13" s="48"/>
-      <x:c r="B13" s="48"/>
-      <x:c r="C13" s="48"/>
-      <x:c r="D13" s="48"/>
-      <x:c r="E13" s="48"/>
-      <x:c r="F13" s="48"/>
+      <x:c r="A13" s="49"/>
+      <x:c r="B13" s="49"/>
+      <x:c r="C13" s="49"/>
+      <x:c r="D13" s="49"/>
+      <x:c r="E13" s="49"/>
+      <x:c r="F13" s="49"/>
     </x:row>
     <x:row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A14" s="38"/>
-      <x:c r="B14" s="38"/>
+      <x:c r="A14" s="52"/>
+      <x:c r="B14" s="52"/>
       <x:c r="C14"/>
-      <x:c r="D14" s="39" t="s">
+      <x:c r="D14" s="41" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E14" s="41"/>
+      <x:c r="F14" s="27" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E14" s="39"/>
-      <x:c r="F14" s="27" t="s">
-        <x:v>13</x:v>
-      </x:c>
     </x:row>
     <x:row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A15" s="38"/>
-      <x:c r="B15" s="38"/>
+      <x:c r="A15" s="52"/>
+      <x:c r="B15" s="52"/>
       <x:c r="C15"/>
-      <x:c r="D15" s="40" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E15" s="40"/>
+      <x:c r="D15" s="38" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E15" s="38"/>
       <x:c r="F15" s="28"/>
     </x:row>
     <x:row r="16" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1067,47 +1250,59 @@
     </x:row>
     <x:row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="27" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B17" s="41" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B17" s="39" t="s">
+      <x:c r="C17" s="41"/>
+      <x:c r="D17" s="41"/>
+      <x:c r="E17" s="27" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C17" s="39"/>
-      <x:c r="D17" s="39"/>
-      <x:c r="E17" s="27" t="s">
+      <x:c r="F17" s="27" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="F17" s="27" t="s">
-        <x:v>17</x:v>
-      </x:c>
     </x:row>
     <x:row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A18" s="29"/>
-      <x:c r="B18" s="43"/>
-      <x:c r="C18" s="40"/>
-      <x:c r="D18" s="40"/>
-      <x:c r="E18" s="31"/>
-      <x:c r="F18" s="32" t="str">
+      <x:c r="A18" s="29">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B18" s="37" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C18" s="38"/>
+      <x:c r="D18" s="38"/>
+      <x:c r="E18" s="31">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="F18" s="32">
         <x:f t="shared" ref="F18:F38" si="0">IF(SUM(A18)&gt;0,SUM(A18*E18),"")</x:f>
-        <x:v/>
+        <x:v>300</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A19" s="30"/>
-      <x:c r="B19" s="41"/>
-      <x:c r="C19" s="42"/>
-      <x:c r="D19" s="42"/>
-      <x:c r="E19" s="33"/>
-      <x:c r="F19" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
+      <x:c r="A19" s="30">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B19" s="39" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C19" s="40"/>
+      <x:c r="D19" s="40"/>
+      <x:c r="E19" s="33">
+        <x:v>600</x:v>
+      </x:c>
+      <x:c r="F19" s="33">
+        <x:f t="shared" si="0"/>
+        <x:v>1200</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="29"/>
-      <x:c r="B20" s="43"/>
-      <x:c r="C20" s="40"/>
-      <x:c r="D20" s="40"/>
+      <x:c r="B20" s="37"/>
+      <x:c r="C20" s="38"/>
+      <x:c r="D20" s="38"/>
       <x:c r="E20" s="34"/>
       <x:c r="F20" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1116,9 +1311,9 @@
     </x:row>
     <x:row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A21" s="30"/>
-      <x:c r="B21" s="41"/>
-      <x:c r="C21" s="42"/>
-      <x:c r="D21" s="42"/>
+      <x:c r="B21" s="39"/>
+      <x:c r="C21" s="40"/>
+      <x:c r="D21" s="40"/>
       <x:c r="E21" s="33"/>
       <x:c r="F21" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1127,9 +1322,9 @@
     </x:row>
     <x:row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A22" s="29"/>
-      <x:c r="B22" s="43"/>
-      <x:c r="C22" s="40"/>
-      <x:c r="D22" s="40"/>
+      <x:c r="B22" s="37"/>
+      <x:c r="C22" s="38"/>
+      <x:c r="D22" s="38"/>
       <x:c r="E22" s="34"/>
       <x:c r="F22" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1138,9 +1333,9 @@
     </x:row>
     <x:row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A23" s="30"/>
-      <x:c r="B23" s="41"/>
-      <x:c r="C23" s="42"/>
-      <x:c r="D23" s="42"/>
+      <x:c r="B23" s="39"/>
+      <x:c r="C23" s="40"/>
+      <x:c r="D23" s="40"/>
       <x:c r="E23" s="33"/>
       <x:c r="F23" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1149,9 +1344,9 @@
     </x:row>
     <x:row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A24" s="29"/>
-      <x:c r="B24" s="43"/>
-      <x:c r="C24" s="40"/>
-      <x:c r="D24" s="40"/>
+      <x:c r="B24" s="37"/>
+      <x:c r="C24" s="38"/>
+      <x:c r="D24" s="38"/>
       <x:c r="E24" s="34"/>
       <x:c r="F24" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1160,9 +1355,9 @@
     </x:row>
     <x:row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="30"/>
-      <x:c r="B25" s="41"/>
-      <x:c r="C25" s="42"/>
-      <x:c r="D25" s="42"/>
+      <x:c r="B25" s="39"/>
+      <x:c r="C25" s="40"/>
+      <x:c r="D25" s="40"/>
       <x:c r="E25" s="33"/>
       <x:c r="F25" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1171,9 +1366,9 @@
     </x:row>
     <x:row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A26" s="29"/>
-      <x:c r="B26" s="43"/>
-      <x:c r="C26" s="40"/>
-      <x:c r="D26" s="40"/>
+      <x:c r="B26" s="37"/>
+      <x:c r="C26" s="38"/>
+      <x:c r="D26" s="38"/>
       <x:c r="E26" s="34"/>
       <x:c r="F26" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1182,9 +1377,9 @@
     </x:row>
     <x:row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A27" s="30"/>
-      <x:c r="B27" s="41"/>
-      <x:c r="C27" s="42"/>
-      <x:c r="D27" s="42"/>
+      <x:c r="B27" s="39"/>
+      <x:c r="C27" s="40"/>
+      <x:c r="D27" s="40"/>
       <x:c r="E27" s="33"/>
       <x:c r="F27" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1193,9 +1388,9 @@
     </x:row>
     <x:row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A28" s="29"/>
-      <x:c r="B28" s="43"/>
-      <x:c r="C28" s="40"/>
-      <x:c r="D28" s="40"/>
+      <x:c r="B28" s="37"/>
+      <x:c r="C28" s="38"/>
+      <x:c r="D28" s="38"/>
       <x:c r="E28" s="34"/>
       <x:c r="F28" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1204,9 +1399,9 @@
     </x:row>
     <x:row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A29" s="30"/>
-      <x:c r="B29" s="41"/>
-      <x:c r="C29" s="42"/>
-      <x:c r="D29" s="42"/>
+      <x:c r="B29" s="39"/>
+      <x:c r="C29" s="40"/>
+      <x:c r="D29" s="40"/>
       <x:c r="E29" s="33"/>
       <x:c r="F29" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1215,9 +1410,9 @@
     </x:row>
     <x:row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A30" s="29"/>
-      <x:c r="B30" s="43"/>
-      <x:c r="C30" s="40"/>
-      <x:c r="D30" s="40"/>
+      <x:c r="B30" s="37"/>
+      <x:c r="C30" s="38"/>
+      <x:c r="D30" s="38"/>
       <x:c r="E30" s="34"/>
       <x:c r="F30" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1226,9 +1421,9 @@
     </x:row>
     <x:row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A31" s="30"/>
-      <x:c r="B31" s="41"/>
-      <x:c r="C31" s="42"/>
-      <x:c r="D31" s="42"/>
+      <x:c r="B31" s="39"/>
+      <x:c r="C31" s="40"/>
+      <x:c r="D31" s="40"/>
       <x:c r="E31" s="33"/>
       <x:c r="F31" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1237,9 +1432,9 @@
     </x:row>
     <x:row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A32" s="29"/>
-      <x:c r="B32" s="43"/>
-      <x:c r="C32" s="40"/>
-      <x:c r="D32" s="40"/>
+      <x:c r="B32" s="37"/>
+      <x:c r="C32" s="38"/>
+      <x:c r="D32" s="38"/>
       <x:c r="E32" s="34"/>
       <x:c r="F32" s="33" t="str">
         <x:f>IF(SUM(A32)&gt;0,SUM(A32*E32),"")</x:f>
@@ -1248,9 +1443,9 @@
     </x:row>
     <x:row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A33" s="30"/>
-      <x:c r="B33" s="41"/>
-      <x:c r="C33" s="42"/>
-      <x:c r="D33" s="42"/>
+      <x:c r="B33" s="39"/>
+      <x:c r="C33" s="40"/>
+      <x:c r="D33" s="40"/>
       <x:c r="E33" s="33"/>
       <x:c r="F33" s="33" t="str">
         <x:f>IF(SUM(A33)&gt;0,SUM(A33*E33),"")</x:f>
@@ -1259,9 +1454,9 @@
     </x:row>
     <x:row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A34" s="29"/>
-      <x:c r="B34" s="43"/>
-      <x:c r="C34" s="40"/>
-      <x:c r="D34" s="40"/>
+      <x:c r="B34" s="37"/>
+      <x:c r="C34" s="38"/>
+      <x:c r="D34" s="38"/>
       <x:c r="E34" s="34"/>
       <x:c r="F34" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1270,9 +1465,9 @@
     </x:row>
     <x:row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A35" s="30"/>
-      <x:c r="B35" s="41"/>
-      <x:c r="C35" s="42"/>
-      <x:c r="D35" s="42"/>
+      <x:c r="B35" s="39"/>
+      <x:c r="C35" s="40"/>
+      <x:c r="D35" s="40"/>
       <x:c r="E35" s="33"/>
       <x:c r="F35" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1281,9 +1476,9 @@
     </x:row>
     <x:row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A36" s="29"/>
-      <x:c r="B36" s="43"/>
-      <x:c r="C36" s="40"/>
-      <x:c r="D36" s="40"/>
+      <x:c r="B36" s="37"/>
+      <x:c r="C36" s="38"/>
+      <x:c r="D36" s="38"/>
       <x:c r="E36" s="34"/>
       <x:c r="F36" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1292,9 +1487,9 @@
     </x:row>
     <x:row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A37" s="30"/>
-      <x:c r="B37" s="41"/>
-      <x:c r="C37" s="42"/>
-      <x:c r="D37" s="42"/>
+      <x:c r="B37" s="39"/>
+      <x:c r="C37" s="40"/>
+      <x:c r="D37" s="40"/>
       <x:c r="E37" s="33"/>
       <x:c r="F37" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1303,9 +1498,9 @@
     </x:row>
     <x:row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A38" s="29"/>
-      <x:c r="B38" s="43"/>
-      <x:c r="C38" s="40"/>
-      <x:c r="D38" s="40"/>
+      <x:c r="B38" s="37"/>
+      <x:c r="C38" s="38"/>
+      <x:c r="D38" s="38"/>
       <x:c r="E38" s="34"/>
       <x:c r="F38" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1318,11 +1513,11 @@
       <x:c r="C39" s="17"/>
       <x:c r="D39" s="17"/>
       <x:c r="E39" s="18" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F39" s="32" t="str">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F39" s="32">
         <x:f>IF(SUM(F18:F38)&gt;0,SUM(F18:F38),"")</x:f>
-        <x:v/>
+        <x:v>1500</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1331,7 +1526,7 @@
       <x:c r="C40" s="17"/>
       <x:c r="D40" s="17"/>
       <x:c r="E40" s="18" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F40" s="34"/>
     </x:row>
@@ -1341,38 +1536,38 @@
       <x:c r="C41" s="17"/>
       <x:c r="D41" s="17"/>
       <x:c r="E41" s="18" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F41" s="35" t="str">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F41" s="35">
         <x:f>IF(SUM(F39)&gt;0,SUM((F39*F40)+F39),"")</x:f>
-        <x:v/>
+        <x:v>1500</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A42" s="49"/>
-      <x:c r="B42" s="49"/>
-      <x:c r="C42" s="49"/>
-      <x:c r="D42" s="49"/>
-      <x:c r="E42" s="49"/>
-      <x:c r="F42" s="49"/>
+      <x:c r="A42" s="43"/>
+      <x:c r="B42" s="43"/>
+      <x:c r="C42" s="43"/>
+      <x:c r="D42" s="43"/>
+      <x:c r="E42" s="43"/>
+      <x:c r="F42" s="43"/>
     </x:row>
     <x:row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A43" s="50" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="B43" s="51"/>
-      <x:c r="C43" s="51"/>
-      <x:c r="D43" s="51"/>
-      <x:c r="E43" s="51"/>
-      <x:c r="F43" s="51"/>
+      <x:c r="A43" s="44" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B43" s="45"/>
+      <x:c r="C43" s="45"/>
+      <x:c r="D43" s="45"/>
+      <x:c r="E43" s="45"/>
+      <x:c r="F43" s="45"/>
     </x:row>
     <x:row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A44" s="51"/>
-      <x:c r="B44" s="51"/>
-      <x:c r="C44" s="51"/>
-      <x:c r="D44" s="51"/>
-      <x:c r="E44" s="51"/>
-      <x:c r="F44" s="51"/>
+      <x:c r="A44" s="45"/>
+      <x:c r="B44" s="45"/>
+      <x:c r="C44" s="45"/>
+      <x:c r="D44" s="45"/>
+      <x:c r="E44" s="45"/>
+      <x:c r="F44" s="45"/>
     </x:row>
     <x:row r="45" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A45" s="19"/>
@@ -1383,14 +1578,14 @@
       <x:c r="F45" s="19"/>
     </x:row>
     <x:row r="46" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A46" s="52" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B46" s="52"/>
-      <x:c r="C46" s="52"/>
-      <x:c r="D46" s="52"/>
-      <x:c r="E46" s="52"/>
-      <x:c r="F46" s="52"/>
+      <x:c r="A46" s="36" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B46" s="36"/>
+      <x:c r="C46" s="36"/>
+      <x:c r="D46" s="36"/>
+      <x:c r="E46" s="36"/>
+      <x:c r="F46" s="36"/>
     </x:row>
     <x:row r="47" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A47" s="21"/>
@@ -1401,10 +1596,10 @@
       <x:c r="F47" s="9"/>
     </x:row>
     <x:row r="48" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="B48" s="36"/>
-      <x:c r="C48" s="37"/>
-      <x:c r="D48" s="37"/>
-      <x:c r="E48" s="37"/>
+      <x:c r="B48" s="50"/>
+      <x:c r="C48" s="51"/>
+      <x:c r="D48" s="51"/>
+      <x:c r="E48" s="51"/>
     </x:row>
     <x:row r="49" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="B49" s="24"/>
@@ -1423,26 +1618,6 @@
     </x:row>
   </x:sheetData>
   <x:mergeCells count="36">
-    <x:mergeCell ref="A46:F46"/>
-    <x:mergeCell ref="B34:D34"/>
-    <x:mergeCell ref="B35:D35"/>
-    <x:mergeCell ref="B31:D31"/>
-    <x:mergeCell ref="B30:D30"/>
-    <x:mergeCell ref="B38:D38"/>
-    <x:mergeCell ref="B37:D37"/>
-    <x:mergeCell ref="B32:D32"/>
-    <x:mergeCell ref="B33:D33"/>
-    <x:mergeCell ref="B19:D19"/>
-    <x:mergeCell ref="B17:D17"/>
-    <x:mergeCell ref="B9:C9"/>
-    <x:mergeCell ref="A42:F42"/>
-    <x:mergeCell ref="A43:F44"/>
-    <x:mergeCell ref="B29:D29"/>
-    <x:mergeCell ref="B1:F1"/>
-    <x:mergeCell ref="A3:C3"/>
-    <x:mergeCell ref="A4:C5"/>
-    <x:mergeCell ref="B8:C8"/>
-    <x:mergeCell ref="A13:F13"/>
     <x:mergeCell ref="B48:E48"/>
     <x:mergeCell ref="A14:B14"/>
     <x:mergeCell ref="A15:B15"/>
@@ -1459,6 +1634,26 @@
     <x:mergeCell ref="B24:D24"/>
     <x:mergeCell ref="B23:D23"/>
     <x:mergeCell ref="B22:D22"/>
+    <x:mergeCell ref="B1:F1"/>
+    <x:mergeCell ref="A3:C3"/>
+    <x:mergeCell ref="A4:C5"/>
+    <x:mergeCell ref="B8:C8"/>
+    <x:mergeCell ref="A13:F13"/>
+    <x:mergeCell ref="B19:D19"/>
+    <x:mergeCell ref="B17:D17"/>
+    <x:mergeCell ref="B9:C9"/>
+    <x:mergeCell ref="A42:F42"/>
+    <x:mergeCell ref="A43:F44"/>
+    <x:mergeCell ref="B29:D29"/>
+    <x:mergeCell ref="A46:F46"/>
+    <x:mergeCell ref="B34:D34"/>
+    <x:mergeCell ref="B35:D35"/>
+    <x:mergeCell ref="B31:D31"/>
+    <x:mergeCell ref="B30:D30"/>
+    <x:mergeCell ref="B38:D38"/>
+    <x:mergeCell ref="B37:D37"/>
+    <x:mergeCell ref="B32:D32"/>
+    <x:mergeCell ref="B33:D33"/>
   </x:mergeCells>
   <x:phoneticPr fontId="1" type="noConversion"/>
   <x:printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Small fixes and examples
</commit_message>
<xml_diff>
--- a/docs/content/SimpleInvoice.xlsx
+++ b/docs/content/SimpleInvoice.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <x:workbookPr/>
   <x:bookViews>
-    <x:workbookView xWindow="-15" yWindow="6165" windowWidth="19170" windowHeight="6225" activeTab="1"/>
+    <x:workbookView xWindow="-15" yWindow="6165" windowWidth="19170" windowHeight="6225"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Service Invoice" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,13 @@
     <x:definedName name="DueDate">'Service Invoice'!$F$15</x:definedName>
     <x:definedName name="InvoiceNumber">'Service Invoice'!$F$4</x:definedName>
     <x:definedName name="Name">'Service Invoice'!$B$8</x:definedName>
-    <x:definedName name="OrderLines">'Service Invoice'!$A$18:$F$38</x:definedName>
     <x:definedName name="PaymentTerms">'Service Invoice'!$D$15</x:definedName>
     <x:definedName name="Phone">'Service Invoice'!$B$12</x:definedName>
     <x:definedName name="_xlnm.Print_Area" localSheetId="0">'Service Invoice'!$A$1:$F$46</x:definedName>
+    <x:definedName name="QTY">'Service Invoice'!$A$18</x:definedName>
     <x:definedName name="SubTotal">'Service Invoice'!$F$39</x:definedName>
     <x:definedName name="Total">'Service Invoice'!$F$41</x:definedName>
+    <x:definedName name="UNITPRICE">'Service Invoice'!$E$18</x:definedName>
     <x:definedName name="VAT">'Service Invoice'!$F$40</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="144525"/>
@@ -419,27 +420,41 @@
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -447,23 +462,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,11 +642,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53420416"/>
-        <c:axId val="53421952"/>
+        <c:axId val="104839040"/>
+        <c:axId val="104840576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53420416"/>
+        <c:axId val="104839040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53421952"/>
+        <c:crossAx val="104840576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53421952"/>
+        <c:axId val="104840576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53420416"/>
+        <c:crossAx val="104839040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -694,7 +695,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="148" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -830,7 +831,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307500" cy="6082500"/>
+    <xdr:ext cx="9306182" cy="6081841"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1082,8 +1083,8 @@
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:dimension ref="A1:F51"/>
   <x:sheetViews>
-    <x:sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <x:selection activeCell="A18" sqref="A18:F19"/>
+    <x:sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <x:selection activeCell="L18" sqref="L18"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1097,13 +1098,13 @@
   <x:sheetData>
     <x:row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="1">
       <x:c r="A1" s="1"/>
-      <x:c r="B1" s="46" t="s">
+      <x:c r="B1" s="44" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C1" s="46"/>
-      <x:c r="D1" s="46"/>
-      <x:c r="E1" s="46"/>
-      <x:c r="F1" s="46"/>
+      <x:c r="C1" s="44"/>
+      <x:c r="D1" s="44"/>
+      <x:c r="E1" s="44"/>
+      <x:c r="F1" s="44"/>
     </x:row>
     <x:row r="2" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A2" s="3"/>
@@ -1114,26 +1115,26 @@
       <x:c r="F2" s="6"/>
     </x:row>
     <x:row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="47" t="s">
+      <x:c r="A3" s="45" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B3" s="47"/>
-      <x:c r="C3" s="47"/>
+      <x:c r="B3" s="45"/>
+      <x:c r="C3" s="45"/>
       <x:c r="D3" s="4"/>
       <x:c r="E3" s="5" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="F3" s="6">
         <x:f ca="1">TODAY()</x:f>
-        <x:v>41892</x:v>
+        <x:v>41908</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="48" t="s">
+      <x:c r="A4" s="46" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B4" s="48"/>
-      <x:c r="C4" s="48"/>
+      <x:c r="B4" s="46"/>
+      <x:c r="C4" s="46"/>
       <x:c r="D4" s="7"/>
       <x:c r="E4" s="5" t="s">
         <x:v>22</x:v>
@@ -1143,9 +1144,9 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="48"/>
-      <x:c r="B5" s="48"/>
-      <x:c r="C5" s="48"/>
+      <x:c r="A5" s="46"/>
+      <x:c r="B5" s="46"/>
+      <x:c r="C5" s="46"/>
       <x:c r="E5" s="5" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -1163,19 +1164,19 @@
       <x:c r="A8" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="B8" s="42" t="s">
+      <x:c r="B8" s="47" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C8" s="42"/>
+      <x:c r="C8" s="47"/>
       <x:c r="E8" s="10"/>
       <x:c r="F8" s="10"/>
     </x:row>
     <x:row r="9" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A9" s="11"/>
-      <x:c r="B9" s="42" t="s">
+      <x:c r="B9" s="47" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C9" s="42"/>
+      <x:c r="C9" s="47"/>
       <x:c r="D9" s="9"/>
       <x:c r="E9" s="10"/>
       <x:c r="F9" s="10"/>
@@ -1211,33 +1212,33 @@
       <x:c r="F12" s="10"/>
     </x:row>
     <x:row r="13" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A13" s="49"/>
-      <x:c r="B13" s="49"/>
-      <x:c r="C13" s="49"/>
-      <x:c r="D13" s="49"/>
-      <x:c r="E13" s="49"/>
-      <x:c r="F13" s="49"/>
+      <x:c r="A13" s="48"/>
+      <x:c r="B13" s="48"/>
+      <x:c r="C13" s="48"/>
+      <x:c r="D13" s="48"/>
+      <x:c r="E13" s="48"/>
+      <x:c r="F13" s="48"/>
     </x:row>
     <x:row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A14" s="52"/>
-      <x:c r="B14" s="52"/>
+      <x:c r="A14" s="38"/>
+      <x:c r="B14" s="38"/>
       <x:c r="C14"/>
-      <x:c r="D14" s="41" t="s">
+      <x:c r="D14" s="39" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E14" s="41"/>
+      <x:c r="E14" s="39"/>
       <x:c r="F14" s="27" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A15" s="52"/>
-      <x:c r="B15" s="52"/>
+      <x:c r="A15" s="38"/>
+      <x:c r="B15" s="38"/>
       <x:c r="C15"/>
-      <x:c r="D15" s="38" t="s">
+      <x:c r="D15" s="40" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="E15" s="38"/>
+      <x:c r="E15" s="40"/>
       <x:c r="F15" s="28"/>
     </x:row>
     <x:row r="16" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1252,11 +1253,11 @@
       <x:c r="A17" s="27" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B17" s="41" t="s">
+      <x:c r="B17" s="39" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C17" s="41"/>
-      <x:c r="D17" s="41"/>
+      <x:c r="C17" s="39"/>
+      <x:c r="D17" s="39"/>
       <x:c r="E17" s="27" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -1268,11 +1269,11 @@
       <x:c r="A18" s="29">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B18" s="37" t="s">
+      <x:c r="B18" s="43" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C18" s="38"/>
-      <x:c r="D18" s="38"/>
+      <x:c r="C18" s="40"/>
+      <x:c r="D18" s="40"/>
       <x:c r="E18" s="31">
         <x:v>300</x:v>
       </x:c>
@@ -1285,11 +1286,11 @@
       <x:c r="A19" s="30">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B19" s="39" t="s">
+      <x:c r="B19" s="41" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C19" s="40"/>
-      <x:c r="D19" s="40"/>
+      <x:c r="C19" s="42"/>
+      <x:c r="D19" s="42"/>
       <x:c r="E19" s="33">
         <x:v>600</x:v>
       </x:c>
@@ -1300,9 +1301,9 @@
     </x:row>
     <x:row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="29"/>
-      <x:c r="B20" s="37"/>
-      <x:c r="C20" s="38"/>
-      <x:c r="D20" s="38"/>
+      <x:c r="B20" s="43"/>
+      <x:c r="C20" s="40"/>
+      <x:c r="D20" s="40"/>
       <x:c r="E20" s="34"/>
       <x:c r="F20" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1311,9 +1312,9 @@
     </x:row>
     <x:row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A21" s="30"/>
-      <x:c r="B21" s="39"/>
-      <x:c r="C21" s="40"/>
-      <x:c r="D21" s="40"/>
+      <x:c r="B21" s="41"/>
+      <x:c r="C21" s="42"/>
+      <x:c r="D21" s="42"/>
       <x:c r="E21" s="33"/>
       <x:c r="F21" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1322,9 +1323,9 @@
     </x:row>
     <x:row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A22" s="29"/>
-      <x:c r="B22" s="37"/>
-      <x:c r="C22" s="38"/>
-      <x:c r="D22" s="38"/>
+      <x:c r="B22" s="43"/>
+      <x:c r="C22" s="40"/>
+      <x:c r="D22" s="40"/>
       <x:c r="E22" s="34"/>
       <x:c r="F22" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1333,9 +1334,9 @@
     </x:row>
     <x:row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A23" s="30"/>
-      <x:c r="B23" s="39"/>
-      <x:c r="C23" s="40"/>
-      <x:c r="D23" s="40"/>
+      <x:c r="B23" s="41"/>
+      <x:c r="C23" s="42"/>
+      <x:c r="D23" s="42"/>
       <x:c r="E23" s="33"/>
       <x:c r="F23" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1344,9 +1345,9 @@
     </x:row>
     <x:row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A24" s="29"/>
-      <x:c r="B24" s="37"/>
-      <x:c r="C24" s="38"/>
-      <x:c r="D24" s="38"/>
+      <x:c r="B24" s="43"/>
+      <x:c r="C24" s="40"/>
+      <x:c r="D24" s="40"/>
       <x:c r="E24" s="34"/>
       <x:c r="F24" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1355,9 +1356,9 @@
     </x:row>
     <x:row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="30"/>
-      <x:c r="B25" s="39"/>
-      <x:c r="C25" s="40"/>
-      <x:c r="D25" s="40"/>
+      <x:c r="B25" s="41"/>
+      <x:c r="C25" s="42"/>
+      <x:c r="D25" s="42"/>
       <x:c r="E25" s="33"/>
       <x:c r="F25" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1366,9 +1367,9 @@
     </x:row>
     <x:row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A26" s="29"/>
-      <x:c r="B26" s="37"/>
-      <x:c r="C26" s="38"/>
-      <x:c r="D26" s="38"/>
+      <x:c r="B26" s="43"/>
+      <x:c r="C26" s="40"/>
+      <x:c r="D26" s="40"/>
       <x:c r="E26" s="34"/>
       <x:c r="F26" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1377,9 +1378,9 @@
     </x:row>
     <x:row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A27" s="30"/>
-      <x:c r="B27" s="39"/>
-      <x:c r="C27" s="40"/>
-      <x:c r="D27" s="40"/>
+      <x:c r="B27" s="41"/>
+      <x:c r="C27" s="42"/>
+      <x:c r="D27" s="42"/>
       <x:c r="E27" s="33"/>
       <x:c r="F27" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1388,9 +1389,9 @@
     </x:row>
     <x:row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A28" s="29"/>
-      <x:c r="B28" s="37"/>
-      <x:c r="C28" s="38"/>
-      <x:c r="D28" s="38"/>
+      <x:c r="B28" s="43"/>
+      <x:c r="C28" s="40"/>
+      <x:c r="D28" s="40"/>
       <x:c r="E28" s="34"/>
       <x:c r="F28" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1399,9 +1400,9 @@
     </x:row>
     <x:row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A29" s="30"/>
-      <x:c r="B29" s="39"/>
-      <x:c r="C29" s="40"/>
-      <x:c r="D29" s="40"/>
+      <x:c r="B29" s="41"/>
+      <x:c r="C29" s="42"/>
+      <x:c r="D29" s="42"/>
       <x:c r="E29" s="33"/>
       <x:c r="F29" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1410,9 +1411,9 @@
     </x:row>
     <x:row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A30" s="29"/>
-      <x:c r="B30" s="37"/>
-      <x:c r="C30" s="38"/>
-      <x:c r="D30" s="38"/>
+      <x:c r="B30" s="43"/>
+      <x:c r="C30" s="40"/>
+      <x:c r="D30" s="40"/>
       <x:c r="E30" s="34"/>
       <x:c r="F30" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1421,9 +1422,9 @@
     </x:row>
     <x:row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A31" s="30"/>
-      <x:c r="B31" s="39"/>
-      <x:c r="C31" s="40"/>
-      <x:c r="D31" s="40"/>
+      <x:c r="B31" s="41"/>
+      <x:c r="C31" s="42"/>
+      <x:c r="D31" s="42"/>
       <x:c r="E31" s="33"/>
       <x:c r="F31" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1432,9 +1433,9 @@
     </x:row>
     <x:row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A32" s="29"/>
-      <x:c r="B32" s="37"/>
-      <x:c r="C32" s="38"/>
-      <x:c r="D32" s="38"/>
+      <x:c r="B32" s="43"/>
+      <x:c r="C32" s="40"/>
+      <x:c r="D32" s="40"/>
       <x:c r="E32" s="34"/>
       <x:c r="F32" s="33" t="str">
         <x:f>IF(SUM(A32)&gt;0,SUM(A32*E32),"")</x:f>
@@ -1443,9 +1444,9 @@
     </x:row>
     <x:row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A33" s="30"/>
-      <x:c r="B33" s="39"/>
-      <x:c r="C33" s="40"/>
-      <x:c r="D33" s="40"/>
+      <x:c r="B33" s="41"/>
+      <x:c r="C33" s="42"/>
+      <x:c r="D33" s="42"/>
       <x:c r="E33" s="33"/>
       <x:c r="F33" s="33" t="str">
         <x:f>IF(SUM(A33)&gt;0,SUM(A33*E33),"")</x:f>
@@ -1454,9 +1455,9 @@
     </x:row>
     <x:row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A34" s="29"/>
-      <x:c r="B34" s="37"/>
-      <x:c r="C34" s="38"/>
-      <x:c r="D34" s="38"/>
+      <x:c r="B34" s="43"/>
+      <x:c r="C34" s="40"/>
+      <x:c r="D34" s="40"/>
       <x:c r="E34" s="34"/>
       <x:c r="F34" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1465,9 +1466,9 @@
     </x:row>
     <x:row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A35" s="30"/>
-      <x:c r="B35" s="39"/>
-      <x:c r="C35" s="40"/>
-      <x:c r="D35" s="40"/>
+      <x:c r="B35" s="41"/>
+      <x:c r="C35" s="42"/>
+      <x:c r="D35" s="42"/>
       <x:c r="E35" s="33"/>
       <x:c r="F35" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1476,9 +1477,9 @@
     </x:row>
     <x:row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A36" s="29"/>
-      <x:c r="B36" s="37"/>
-      <x:c r="C36" s="38"/>
-      <x:c r="D36" s="38"/>
+      <x:c r="B36" s="43"/>
+      <x:c r="C36" s="40"/>
+      <x:c r="D36" s="40"/>
       <x:c r="E36" s="34"/>
       <x:c r="F36" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1487,9 +1488,9 @@
     </x:row>
     <x:row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A37" s="30"/>
-      <x:c r="B37" s="39"/>
-      <x:c r="C37" s="40"/>
-      <x:c r="D37" s="40"/>
+      <x:c r="B37" s="41"/>
+      <x:c r="C37" s="42"/>
+      <x:c r="D37" s="42"/>
       <x:c r="E37" s="33"/>
       <x:c r="F37" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1498,9 +1499,9 @@
     </x:row>
     <x:row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A38" s="29"/>
-      <x:c r="B38" s="37"/>
-      <x:c r="C38" s="38"/>
-      <x:c r="D38" s="38"/>
+      <x:c r="B38" s="43"/>
+      <x:c r="C38" s="40"/>
+      <x:c r="D38" s="40"/>
       <x:c r="E38" s="34"/>
       <x:c r="F38" s="33" t="str">
         <x:f t="shared" si="0"/>
@@ -1544,30 +1545,30 @@
       </x:c>
     </x:row>
     <x:row r="42" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A42" s="43"/>
-      <x:c r="B42" s="43"/>
-      <x:c r="C42" s="43"/>
-      <x:c r="D42" s="43"/>
-      <x:c r="E42" s="43"/>
-      <x:c r="F42" s="43"/>
+      <x:c r="A42" s="49"/>
+      <x:c r="B42" s="49"/>
+      <x:c r="C42" s="49"/>
+      <x:c r="D42" s="49"/>
+      <x:c r="E42" s="49"/>
+      <x:c r="F42" s="49"/>
     </x:row>
     <x:row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A43" s="44" t="s">
+      <x:c r="A43" s="50" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B43" s="45"/>
-      <x:c r="C43" s="45"/>
-      <x:c r="D43" s="45"/>
-      <x:c r="E43" s="45"/>
-      <x:c r="F43" s="45"/>
+      <x:c r="B43" s="51"/>
+      <x:c r="C43" s="51"/>
+      <x:c r="D43" s="51"/>
+      <x:c r="E43" s="51"/>
+      <x:c r="F43" s="51"/>
     </x:row>
     <x:row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A44" s="45"/>
-      <x:c r="B44" s="45"/>
-      <x:c r="C44" s="45"/>
-      <x:c r="D44" s="45"/>
-      <x:c r="E44" s="45"/>
-      <x:c r="F44" s="45"/>
+      <x:c r="A44" s="51"/>
+      <x:c r="B44" s="51"/>
+      <x:c r="C44" s="51"/>
+      <x:c r="D44" s="51"/>
+      <x:c r="E44" s="51"/>
+      <x:c r="F44" s="51"/>
     </x:row>
     <x:row r="45" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A45" s="19"/>
@@ -1578,14 +1579,14 @@
       <x:c r="F45" s="19"/>
     </x:row>
     <x:row r="46" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A46" s="36" t="s">
+      <x:c r="A46" s="52" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B46" s="36"/>
-      <x:c r="C46" s="36"/>
-      <x:c r="D46" s="36"/>
-      <x:c r="E46" s="36"/>
-      <x:c r="F46" s="36"/>
+      <x:c r="B46" s="52"/>
+      <x:c r="C46" s="52"/>
+      <x:c r="D46" s="52"/>
+      <x:c r="E46" s="52"/>
+      <x:c r="F46" s="52"/>
     </x:row>
     <x:row r="47" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A47" s="21"/>
@@ -1596,10 +1597,10 @@
       <x:c r="F47" s="9"/>
     </x:row>
     <x:row r="48" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="B48" s="50"/>
-      <x:c r="C48" s="51"/>
-      <x:c r="D48" s="51"/>
-      <x:c r="E48" s="51"/>
+      <x:c r="B48" s="36"/>
+      <x:c r="C48" s="37"/>
+      <x:c r="D48" s="37"/>
+      <x:c r="E48" s="37"/>
     </x:row>
     <x:row r="49" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="B49" s="24"/>
@@ -1618,6 +1619,26 @@
     </x:row>
   </x:sheetData>
   <x:mergeCells count="36">
+    <x:mergeCell ref="A46:F46"/>
+    <x:mergeCell ref="B34:D34"/>
+    <x:mergeCell ref="B35:D35"/>
+    <x:mergeCell ref="B31:D31"/>
+    <x:mergeCell ref="B30:D30"/>
+    <x:mergeCell ref="B38:D38"/>
+    <x:mergeCell ref="B37:D37"/>
+    <x:mergeCell ref="B32:D32"/>
+    <x:mergeCell ref="B33:D33"/>
+    <x:mergeCell ref="B19:D19"/>
+    <x:mergeCell ref="B17:D17"/>
+    <x:mergeCell ref="B9:C9"/>
+    <x:mergeCell ref="A42:F42"/>
+    <x:mergeCell ref="A43:F44"/>
+    <x:mergeCell ref="B29:D29"/>
+    <x:mergeCell ref="B1:F1"/>
+    <x:mergeCell ref="A3:C3"/>
+    <x:mergeCell ref="A4:C5"/>
+    <x:mergeCell ref="B8:C8"/>
+    <x:mergeCell ref="A13:F13"/>
     <x:mergeCell ref="B48:E48"/>
     <x:mergeCell ref="A14:B14"/>
     <x:mergeCell ref="A15:B15"/>
@@ -1634,26 +1655,6 @@
     <x:mergeCell ref="B24:D24"/>
     <x:mergeCell ref="B23:D23"/>
     <x:mergeCell ref="B22:D22"/>
-    <x:mergeCell ref="B1:F1"/>
-    <x:mergeCell ref="A3:C3"/>
-    <x:mergeCell ref="A4:C5"/>
-    <x:mergeCell ref="B8:C8"/>
-    <x:mergeCell ref="A13:F13"/>
-    <x:mergeCell ref="B19:D19"/>
-    <x:mergeCell ref="B17:D17"/>
-    <x:mergeCell ref="B9:C9"/>
-    <x:mergeCell ref="A42:F42"/>
-    <x:mergeCell ref="A43:F44"/>
-    <x:mergeCell ref="B29:D29"/>
-    <x:mergeCell ref="A46:F46"/>
-    <x:mergeCell ref="B34:D34"/>
-    <x:mergeCell ref="B35:D35"/>
-    <x:mergeCell ref="B31:D31"/>
-    <x:mergeCell ref="B30:D30"/>
-    <x:mergeCell ref="B38:D38"/>
-    <x:mergeCell ref="B37:D37"/>
-    <x:mergeCell ref="B32:D32"/>
-    <x:mergeCell ref="B33:D33"/>
   </x:mergeCells>
   <x:phoneticPr fontId="1" type="noConversion"/>
   <x:printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Type inference sort of working..
</commit_message>
<xml_diff>
--- a/docs/content/SimpleInvoice.xlsx
+++ b/docs/content/SimpleInvoice.xlsx
@@ -1,40 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <x:workbookPr/>
-  <x:bookViews>
-    <x:workbookView xWindow="-15" yWindow="6165" windowWidth="19170" windowHeight="6225"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Service Invoice" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Chart1" sheetId="3" r:id="rId2"/>
-  </x:sheets>
-  <x:definedNames>
-    <x:definedName name="Address2">'Service Invoice'!$B$11</x:definedName>
-    <x:definedName name="CompanyName">'Service Invoice'!$B$9</x:definedName>
-    <x:definedName name="Date">'Service Invoice'!$F$3</x:definedName>
-    <x:definedName name="DueDate">'Service Invoice'!$F$15</x:definedName>
-    <x:definedName name="InvoiceNumber">'Service Invoice'!$F$4</x:definedName>
-    <x:definedName name="Name">'Service Invoice'!$B$8</x:definedName>
-    <x:definedName name="PaymentTerms">'Service Invoice'!$D$15</x:definedName>
-    <x:definedName name="Phone">'Service Invoice'!$B$12</x:definedName>
-    <x:definedName name="_xlnm.Print_Area" localSheetId="0">'Service Invoice'!$A$1:$F$46</x:definedName>
-    <x:definedName name="QTY">'Service Invoice'!$A$18</x:definedName>
-    <x:definedName name="SubTotal">'Service Invoice'!$F$39</x:definedName>
-    <x:definedName name="Total">'Service Invoice'!$F$41</x:definedName>
-    <x:definedName name="UNITPRICE">'Service Invoice'!$E$18</x:definedName>
-    <x:definedName name="VAT">'Service Invoice'!$F$40</x:definedName>
-  </x:definedNames>
-  <x:calcPr calcId="144525"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinbull/Appdev/officeprovider/docs/content/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="6160" windowWidth="28880" windowHeight="12420"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Service Invoice" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="3" r:id="rId2"/>
+  </sheets>
+  <definedNames>
+    <definedName name="Address2">'Service Invoice'!$B$11</definedName>
+    <definedName name="CompanyName">'Service Invoice'!$B$9</definedName>
+    <definedName name="Date">'Service Invoice'!$F$3</definedName>
+    <definedName name="DueDate">'Service Invoice'!$F$15</definedName>
+    <definedName name="InvoiceNumber">'Service Invoice'!$F$4</definedName>
+    <definedName name="Name">'Service Invoice'!$B$8</definedName>
+    <definedName name="PaymentTerms">'Service Invoice'!$D$15</definedName>
+    <definedName name="Phone">'Service Invoice'!$B$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Service Invoice'!$A$1:$F$46</definedName>
+    <definedName name="QTY">'Service Invoice'!$A$18</definedName>
+    <definedName name="SubTotal">'Service Invoice'!$F$39</definedName>
+    <definedName name="Total">'Service Invoice'!$F$41</definedName>
+    <definedName name="UNITPRICE">'Service Invoice'!$E$18</definedName>
+    <definedName name="VAT">'Service Invoice'!$F$40</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>[100]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>[Company Name]</t>
   </si>
@@ -154,10 +161,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -342,7 +349,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -396,7 +403,7 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -411,50 +418,36 @@
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,9 +455,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,9 +585,12 @@
             <c:strRef>
               <c:f>'Service Invoice'!$A$18:$B$18</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.00 FooBar</c:v>
+                  <c:v>1.00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FooBar</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -593,10 +603,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="2" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -609,9 +619,12 @@
             <c:strRef>
               <c:f>'Service Invoice'!$A$19:$B$19</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2.00 FooBar 2</c:v>
+                  <c:v>2.00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FooBar 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -624,10 +637,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="2" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
-                  <c:v>600</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
-                  <c:v>1200</c:v>
+                  <c:v>1200.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,11 +655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104839040"/>
-        <c:axId val="104840576"/>
+        <c:axId val="-2139980608"/>
+        <c:axId val="-2139984224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104839040"/>
+        <c:axId val="-2139980608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,7 +668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104840576"/>
+        <c:crossAx val="-2139984224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -663,7 +676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104840576"/>
+        <c:axId val="-2139984224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,14 +687,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104839040"/>
+        <c:crossAx val="-2139980608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1080,589 +1092,589 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:dimension ref="A1:F51"/>
-  <x:sheetViews>
-    <x:sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <x:selection activeCell="L18" sqref="L18"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
-  <x:cols>
-    <x:col min="1" max="2" width="13.7109375" style="2" customWidth="1"/>
-    <x:col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
-    <x:col min="4" max="5" width="13.7109375" style="2" customWidth="1"/>
-    <x:col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
-    <x:col min="7" max="16384" width="9.140625" style="2"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="1">
-      <x:c r="A1" s="1"/>
-      <x:c r="B1" s="44" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C1" s="44"/>
-      <x:c r="D1" s="44"/>
-      <x:c r="E1" s="44"/>
-      <x:c r="F1" s="44"/>
-    </x:row>
-    <x:row r="2" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A2" s="3"/>
-      <x:c r="B2" s="3"/>
-      <x:c r="C2" s="3"/>
-      <x:c r="D2" s="4"/>
-      <x:c r="E2" s="5"/>
-      <x:c r="F2" s="6"/>
-    </x:row>
-    <x:row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="45" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B3" s="45"/>
-      <x:c r="C3" s="45"/>
-      <x:c r="D3" s="4"/>
-      <x:c r="E3" s="5" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F3" s="6">
-        <x:f ca="1">TODAY()</x:f>
-        <x:v>41908</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="46" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B4" s="46"/>
-      <x:c r="C4" s="46"/>
-      <x:c r="D4" s="7"/>
-      <x:c r="E4" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="F4" s="5" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="46"/>
-      <x:c r="B5" s="46"/>
-      <x:c r="C5" s="46"/>
-      <x:c r="E5" s="5" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F5" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="F6" s="9"/>
-    </x:row>
-    <x:row r="7" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="F7" s="10"/>
-    </x:row>
-    <x:row r="8" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A8" s="5" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B8" s="47" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C8" s="47"/>
-      <x:c r="E8" s="10"/>
-      <x:c r="F8" s="10"/>
-    </x:row>
-    <x:row r="9" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A9" s="11"/>
-      <x:c r="B9" s="47" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C9" s="47"/>
-      <x:c r="D9" s="9"/>
-      <x:c r="E9" s="10"/>
-      <x:c r="F9" s="10"/>
-    </x:row>
-    <x:row r="10" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A10" s="9"/>
-      <x:c r="B10" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C10" s="5"/>
-      <x:c r="D10" s="9"/>
-      <x:c r="E10" s="10"/>
-      <x:c r="F10" s="10"/>
-    </x:row>
-    <x:row r="11" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A11" s="9"/>
-      <x:c r="B11" s="5" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C11" s="5"/>
-      <x:c r="D11" s="5"/>
-      <x:c r="E11" s="10"/>
-      <x:c r="F11" s="10"/>
-    </x:row>
-    <x:row r="12" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A12" s="9"/>
-      <x:c r="B12" s="5" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C12" s="5"/>
-      <x:c r="D12" s="9"/>
-      <x:c r="E12" s="10"/>
-      <x:c r="F12" s="10"/>
-    </x:row>
-    <x:row r="13" spans="1:6" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A13" s="48"/>
-      <x:c r="B13" s="48"/>
-      <x:c r="C13" s="48"/>
-      <x:c r="D13" s="48"/>
-      <x:c r="E13" s="48"/>
-      <x:c r="F13" s="48"/>
-    </x:row>
-    <x:row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A14" s="38"/>
-      <x:c r="B14" s="38"/>
-      <x:c r="C14"/>
-      <x:c r="D14" s="39" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E14" s="39"/>
-      <x:c r="F14" s="27" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A15" s="38"/>
-      <x:c r="B15" s="38"/>
-      <x:c r="C15"/>
-      <x:c r="D15" s="40" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E15" s="40"/>
-      <x:c r="F15" s="28"/>
-    </x:row>
-    <x:row r="16" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A16" s="12"/>
-      <x:c r="B16" s="12"/>
-      <x:c r="C16" s="13"/>
-      <x:c r="D16" s="13"/>
-      <x:c r="E16" s="13"/>
-      <x:c r="F16" s="14"/>
-    </x:row>
-    <x:row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A17" s="27" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B17" s="39" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C17" s="39"/>
-      <x:c r="D17" s="39"/>
-      <x:c r="E17" s="27" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="F17" s="27" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A18" s="29">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B18" s="43" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C18" s="40"/>
-      <x:c r="D18" s="40"/>
-      <x:c r="E18" s="31">
-        <x:v>300</x:v>
-      </x:c>
-      <x:c r="F18" s="32">
-        <x:f t="shared" ref="F18:F38" si="0">IF(SUM(A18)&gt;0,SUM(A18*E18),"")</x:f>
-        <x:v>300</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A19" s="30">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B19" s="41" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C19" s="42"/>
-      <x:c r="D19" s="42"/>
-      <x:c r="E19" s="33">
-        <x:v>600</x:v>
-      </x:c>
-      <x:c r="F19" s="33">
-        <x:f t="shared" si="0"/>
-        <x:v>1200</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A20" s="29"/>
-      <x:c r="B20" s="43"/>
-      <x:c r="C20" s="40"/>
-      <x:c r="D20" s="40"/>
-      <x:c r="E20" s="34"/>
-      <x:c r="F20" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A21" s="30"/>
-      <x:c r="B21" s="41"/>
-      <x:c r="C21" s="42"/>
-      <x:c r="D21" s="42"/>
-      <x:c r="E21" s="33"/>
-      <x:c r="F21" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A22" s="29"/>
-      <x:c r="B22" s="43"/>
-      <x:c r="C22" s="40"/>
-      <x:c r="D22" s="40"/>
-      <x:c r="E22" s="34"/>
-      <x:c r="F22" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A23" s="30"/>
-      <x:c r="B23" s="41"/>
-      <x:c r="C23" s="42"/>
-      <x:c r="D23" s="42"/>
-      <x:c r="E23" s="33"/>
-      <x:c r="F23" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A24" s="29"/>
-      <x:c r="B24" s="43"/>
-      <x:c r="C24" s="40"/>
-      <x:c r="D24" s="40"/>
-      <x:c r="E24" s="34"/>
-      <x:c r="F24" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A25" s="30"/>
-      <x:c r="B25" s="41"/>
-      <x:c r="C25" s="42"/>
-      <x:c r="D25" s="42"/>
-      <x:c r="E25" s="33"/>
-      <x:c r="F25" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A26" s="29"/>
-      <x:c r="B26" s="43"/>
-      <x:c r="C26" s="40"/>
-      <x:c r="D26" s="40"/>
-      <x:c r="E26" s="34"/>
-      <x:c r="F26" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A27" s="30"/>
-      <x:c r="B27" s="41"/>
-      <x:c r="C27" s="42"/>
-      <x:c r="D27" s="42"/>
-      <x:c r="E27" s="33"/>
-      <x:c r="F27" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A28" s="29"/>
-      <x:c r="B28" s="43"/>
-      <x:c r="C28" s="40"/>
-      <x:c r="D28" s="40"/>
-      <x:c r="E28" s="34"/>
-      <x:c r="F28" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A29" s="30"/>
-      <x:c r="B29" s="41"/>
-      <x:c r="C29" s="42"/>
-      <x:c r="D29" s="42"/>
-      <x:c r="E29" s="33"/>
-      <x:c r="F29" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A30" s="29"/>
-      <x:c r="B30" s="43"/>
-      <x:c r="C30" s="40"/>
-      <x:c r="D30" s="40"/>
-      <x:c r="E30" s="34"/>
-      <x:c r="F30" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A31" s="30"/>
-      <x:c r="B31" s="41"/>
-      <x:c r="C31" s="42"/>
-      <x:c r="D31" s="42"/>
-      <x:c r="E31" s="33"/>
-      <x:c r="F31" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A32" s="29"/>
-      <x:c r="B32" s="43"/>
-      <x:c r="C32" s="40"/>
-      <x:c r="D32" s="40"/>
-      <x:c r="E32" s="34"/>
-      <x:c r="F32" s="33" t="str">
-        <x:f>IF(SUM(A32)&gt;0,SUM(A32*E32),"")</x:f>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A33" s="30"/>
-      <x:c r="B33" s="41"/>
-      <x:c r="C33" s="42"/>
-      <x:c r="D33" s="42"/>
-      <x:c r="E33" s="33"/>
-      <x:c r="F33" s="33" t="str">
-        <x:f>IF(SUM(A33)&gt;0,SUM(A33*E33),"")</x:f>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A34" s="29"/>
-      <x:c r="B34" s="43"/>
-      <x:c r="C34" s="40"/>
-      <x:c r="D34" s="40"/>
-      <x:c r="E34" s="34"/>
-      <x:c r="F34" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A35" s="30"/>
-      <x:c r="B35" s="41"/>
-      <x:c r="C35" s="42"/>
-      <x:c r="D35" s="42"/>
-      <x:c r="E35" s="33"/>
-      <x:c r="F35" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A36" s="29"/>
-      <x:c r="B36" s="43"/>
-      <x:c r="C36" s="40"/>
-      <x:c r="D36" s="40"/>
-      <x:c r="E36" s="34"/>
-      <x:c r="F36" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A37" s="30"/>
-      <x:c r="B37" s="41"/>
-      <x:c r="C37" s="42"/>
-      <x:c r="D37" s="42"/>
-      <x:c r="E37" s="33"/>
-      <x:c r="F37" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A38" s="29"/>
-      <x:c r="B38" s="43"/>
-      <x:c r="C38" s="40"/>
-      <x:c r="D38" s="40"/>
-      <x:c r="E38" s="34"/>
-      <x:c r="F38" s="33" t="str">
-        <x:f t="shared" si="0"/>
-        <x:v/>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A39" s="16"/>
-      <x:c r="B39" s="17"/>
-      <x:c r="C39" s="17"/>
-      <x:c r="D39" s="17"/>
-      <x:c r="E39" s="18" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F39" s="32">
-        <x:f>IF(SUM(F18:F38)&gt;0,SUM(F18:F38),"")</x:f>
-        <x:v>1500</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A40" s="17"/>
-      <x:c r="B40" s="17"/>
-      <x:c r="C40" s="17"/>
-      <x:c r="D40" s="17"/>
-      <x:c r="E40" s="18" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F40" s="34"/>
-    </x:row>
-    <x:row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A41" s="17"/>
-      <x:c r="B41" s="17"/>
-      <x:c r="C41" s="17"/>
-      <x:c r="D41" s="17"/>
-      <x:c r="E41" s="18" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="F41" s="35">
-        <x:f>IF(SUM(F39)&gt;0,SUM((F39*F40)+F39),"")</x:f>
-        <x:v>1500</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A42" s="49"/>
-      <x:c r="B42" s="49"/>
-      <x:c r="C42" s="49"/>
-      <x:c r="D42" s="49"/>
-      <x:c r="E42" s="49"/>
-      <x:c r="F42" s="49"/>
-    </x:row>
-    <x:row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A43" s="50" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B43" s="51"/>
-      <x:c r="C43" s="51"/>
-      <x:c r="D43" s="51"/>
-      <x:c r="E43" s="51"/>
-      <x:c r="F43" s="51"/>
-    </x:row>
-    <x:row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A44" s="51"/>
-      <x:c r="B44" s="51"/>
-      <x:c r="C44" s="51"/>
-      <x:c r="D44" s="51"/>
-      <x:c r="E44" s="51"/>
-      <x:c r="F44" s="51"/>
-    </x:row>
-    <x:row r="45" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A45" s="19"/>
-      <x:c r="B45" s="19"/>
-      <x:c r="C45" s="19"/>
-      <x:c r="D45" s="19"/>
-      <x:c r="E45" s="19"/>
-      <x:c r="F45" s="19"/>
-    </x:row>
-    <x:row r="46" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A46" s="52" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B46" s="52"/>
-      <x:c r="C46" s="52"/>
-      <x:c r="D46" s="52"/>
-      <x:c r="E46" s="52"/>
-      <x:c r="F46" s="52"/>
-    </x:row>
-    <x:row r="47" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A47" s="21"/>
-      <x:c r="B47" s="22"/>
-      <x:c r="C47" s="22"/>
-      <x:c r="D47" s="23"/>
-      <x:c r="E47" s="9"/>
-      <x:c r="F47" s="9"/>
-    </x:row>
-    <x:row r="48" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="B48" s="36"/>
-      <x:c r="C48" s="37"/>
-      <x:c r="D48" s="37"/>
-      <x:c r="E48" s="37"/>
-    </x:row>
-    <x:row r="49" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="B49" s="24"/>
-      <x:c r="C49" s="25"/>
-      <x:c r="D49" s="25"/>
-      <x:c r="E49" s="25"/>
-    </x:row>
-    <x:row r="50" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <x:row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <x:c r="A51" s="26"/>
-      <x:c r="B51" s="26"/>
-      <x:c r="C51" s="26"/>
-      <x:c r="D51" s="26"/>
-      <x:c r="E51" s="26"/>
-      <x:c r="F51" s="26"/>
-    </x:row>
-  </x:sheetData>
-  <x:mergeCells count="36">
-    <x:mergeCell ref="A46:F46"/>
-    <x:mergeCell ref="B34:D34"/>
-    <x:mergeCell ref="B35:D35"/>
-    <x:mergeCell ref="B31:D31"/>
-    <x:mergeCell ref="B30:D30"/>
-    <x:mergeCell ref="B38:D38"/>
-    <x:mergeCell ref="B37:D37"/>
-    <x:mergeCell ref="B32:D32"/>
-    <x:mergeCell ref="B33:D33"/>
-    <x:mergeCell ref="B19:D19"/>
-    <x:mergeCell ref="B17:D17"/>
-    <x:mergeCell ref="B9:C9"/>
-    <x:mergeCell ref="A42:F42"/>
-    <x:mergeCell ref="A43:F44"/>
-    <x:mergeCell ref="B29:D29"/>
-    <x:mergeCell ref="B1:F1"/>
-    <x:mergeCell ref="A3:C3"/>
-    <x:mergeCell ref="A4:C5"/>
-    <x:mergeCell ref="B8:C8"/>
-    <x:mergeCell ref="A13:F13"/>
-    <x:mergeCell ref="B48:E48"/>
-    <x:mergeCell ref="A14:B14"/>
-    <x:mergeCell ref="A15:B15"/>
-    <x:mergeCell ref="D14:E14"/>
-    <x:mergeCell ref="D15:E15"/>
-    <x:mergeCell ref="B21:D21"/>
-    <x:mergeCell ref="B20:D20"/>
-    <x:mergeCell ref="B36:D36"/>
-    <x:mergeCell ref="B18:D18"/>
-    <x:mergeCell ref="B28:D28"/>
-    <x:mergeCell ref="B27:D27"/>
-    <x:mergeCell ref="B26:D26"/>
-    <x:mergeCell ref="B25:D25"/>
-    <x:mergeCell ref="B24:D24"/>
-    <x:mergeCell ref="B23:D23"/>
-    <x:mergeCell ref="B22:D22"/>
-  </x:mergeCells>
-  <x:phoneticPr fontId="1" type="noConversion"/>
-  <x:printOptions horizontalCentered="1"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <x:pageSetup orientation="portrait" r:id="rId1"/>
-  <x:headerFooter alignWithMargins="0"/>
-  <x:drawing r:id="rId2"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="13.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="13.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="1"/>
+      <c r="B1" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6">
+        <f ca="1">TODAY()</f>
+        <v>42499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="11"/>
+      <c r="B9" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="42"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9"/>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14"/>
+      <c r="D14" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15"/>
+      <c r="D15" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="16" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="29">
+        <v>1</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="31">
+        <v>300</v>
+      </c>
+      <c r="F18" s="32">
+        <f t="shared" ref="F18:F38" si="0">IF(SUM(A18)&gt;0,SUM(A18*E18),"")</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="30">
+        <v>2</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="33">
+        <v>600</v>
+      </c>
+      <c r="F19" s="33">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="29"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="30"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="30"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="30"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="29"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="30"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="29"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="30"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="29"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="30"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="29"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="33" t="str">
+        <f>IF(SUM(A32)&gt;0,SUM(A32*E32),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="30"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33" t="str">
+        <f>IF(SUM(A33)&gt;0,SUM(A33*E33),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="29"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="30"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="29"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="30"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="29"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="32">
+        <f>IF(SUM(F18:F38)&gt;0,SUM(F18:F38),"")</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="34"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="35">
+        <f>IF(SUM(F39)&gt;0,SUM((F39*F40)+F39),"")</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+    </row>
+    <row r="45" spans="1:6" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+    </row>
+    <row r="46" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+    </row>
+    <row r="47" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="21"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="50"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+    </row>
+    <row r="49" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="24"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+    </row>
+    <row r="50" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F44"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>